<commit_message>
Minh chua lam phan bien ban hop. Se update som.
</commit_message>
<xml_diff>
--- a/ProjectDocuments/Nhom14/Template_BangDanhGiaThanhVien.xlsx
+++ b/ProjectDocuments/Nhom14/Template_BangDanhGiaThanhVien.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>BẢNG ĐÁNH GIÁ THÀNH VIÊN</t>
   </si>
@@ -88,6 +88,36 @@
   </si>
   <si>
     <t>Phân công 7</t>
+  </si>
+  <si>
+    <t>0712152</t>
+  </si>
+  <si>
+    <t>Lê Long Hồ</t>
+  </si>
+  <si>
+    <t>0712163</t>
+  </si>
+  <si>
+    <t>Võ Minh Hiển</t>
+  </si>
+  <si>
+    <t>0712174</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Hiếu</t>
+  </si>
+  <si>
+    <t>0712178</t>
+  </si>
+  <si>
+    <t>Nguyễn Ngọc Hoà</t>
+  </si>
+  <si>
+    <t>0712190</t>
+  </si>
+  <si>
+    <t>Lê Gia Quốc Huy</t>
   </si>
 </sst>
 </file>
@@ -201,7 +231,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -245,6 +275,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -545,7 +576,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -880,75 +911,165 @@
       <c r="B19" s="3">
         <v>1</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="C19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="17">
+        <v>1</v>
+      </c>
+      <c r="F19" s="17">
+        <v>1</v>
+      </c>
+      <c r="G19" s="17">
+        <v>1</v>
+      </c>
+      <c r="H19" s="17">
+        <v>1</v>
+      </c>
+      <c r="I19" s="17">
+        <v>1</v>
+      </c>
+      <c r="J19" s="17">
+        <v>1</v>
+      </c>
+      <c r="K19" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="16"/>
       <c r="B20" s="3">
         <v>2</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="C20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="17">
+        <v>1</v>
+      </c>
+      <c r="F20" s="17">
+        <v>1</v>
+      </c>
+      <c r="G20" s="17">
+        <v>1</v>
+      </c>
+      <c r="H20" s="17">
+        <v>1</v>
+      </c>
+      <c r="I20" s="17">
+        <v>1</v>
+      </c>
+      <c r="J20" s="17">
+        <v>1</v>
+      </c>
+      <c r="K20" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="16"/>
       <c r="B21" s="3">
         <v>3</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="C21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="17">
+        <v>1</v>
+      </c>
+      <c r="G21" s="17">
+        <v>1</v>
+      </c>
+      <c r="H21" s="17">
+        <v>1</v>
+      </c>
+      <c r="I21" s="17">
+        <v>1</v>
+      </c>
+      <c r="J21" s="17">
+        <v>1</v>
+      </c>
+      <c r="K21" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="16"/>
       <c r="B22" s="3">
         <v>4</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="C22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="17">
+        <v>1</v>
+      </c>
+      <c r="F22" s="17">
+        <v>1</v>
+      </c>
+      <c r="G22" s="17">
+        <v>1</v>
+      </c>
+      <c r="H22" s="17">
+        <v>1</v>
+      </c>
+      <c r="I22" s="17">
+        <v>1</v>
+      </c>
+      <c r="J22" s="17">
+        <v>1</v>
+      </c>
+      <c r="K22" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="16"/>
       <c r="B23" s="3">
         <v>5</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="C23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="17">
+        <v>1</v>
+      </c>
+      <c r="F23" s="17">
+        <v>1</v>
+      </c>
+      <c r="G23" s="17">
+        <v>1</v>
+      </c>
+      <c r="H23" s="17">
+        <v>1</v>
+      </c>
+      <c r="I23" s="17">
+        <v>1</v>
+      </c>
+      <c r="J23" s="17">
+        <v>1</v>
+      </c>
+      <c r="K23" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="14">

</xml_diff>